<commit_message>
Perfected Excel export and import functionality for seamless data management.
</commit_message>
<xml_diff>
--- a/test_patient_import.xlsx
+++ b/test_patient_import.xlsx
@@ -397,18 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
-    <col min="4" max="4" width="50.83203125" customWidth="1"/>
-    <col min="5" max="5" width="60.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -441,10 +433,10 @@
         <v>Persistent sadness and loss of interest in activities</v>
       </c>
       <c r="D2" t="str">
-        <v>Patient presents with 3-month history of depressed mood, decreased appetite, and insomnia</v>
+        <v>Patient presents with 3-month history of depressed mood</v>
       </c>
       <c r="E2" t="str">
-        <v>Patient is a 35-year-old male with major depressive disorder. Reports feeling sad most days, has lost interest in hobbies, experiencing sleep difficulties.</v>
+        <v>Patient is a 35-year-old male with major depressive disorder</v>
       </c>
       <c r="F2" t="str">
         <v>active</v>
@@ -461,10 +453,10 @@
         <v>Anxiety and panic attacks</v>
       </c>
       <c r="D3" t="str">
-        <v>Patient reports increasing anxiety over past 6 months with frequent panic attacks</v>
+        <v>Patient reports increasing anxiety over past 6 months</v>
       </c>
       <c r="E3" t="str">
-        <v>Patient is a 28-year-old female with generalized anxiety disorder. Experiences excessive worry, physical tension, and occasional panic attacks.</v>
+        <v>Patient is a 28-year-old female with generalized anxiety disorder</v>
       </c>
       <c r="F3" t="str">
         <v>active</v>
@@ -481,58 +473,18 @@
         <v>Sleep disturbances and racing thoughts</v>
       </c>
       <c r="D4" t="str">
-        <v>Patient describes alternating periods of high and low mood with associated sleep changes</v>
+        <v>Patient describes alternating periods of high and low mood</v>
       </c>
       <c r="E4" t="str">
-        <v>Patient is a 42-year-old male with bipolar disorder. Currently in depressive phase with history of manic episodes.</v>
+        <v>Patient is a 42-year-old male with bipolar disorder</v>
       </c>
       <c r="F4" t="str">
         <v>follow_up</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sarah</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Williams</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Intrusive thoughts and compulsive behaviors</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Patient reports distressing intrusive thoughts and time-consuming rituals</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Patient is a 31-year-old female with OCD. Spends several hours daily on checking and cleaning rituals.</v>
-      </c>
-      <c r="F5" t="str">
-        <v>active</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Robert</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Brown</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Social withdrawal and flat affect</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Family reports patient has been increasingly isolated with blunted emotional expression</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Patient is a 26-year-old male with schizophrenia spectrum disorder. Presents with negative symptoms and social dysfunction.</v>
-      </c>
-      <c r="F6" t="str">
-        <v>active</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>